<commit_message>
AnalysisTemplate columns have been re-organized.
</commit_message>
<xml_diff>
--- a/AnalysisTemplate.xlsx
+++ b/AnalysisTemplate.xlsx
@@ -234,7 +234,7 @@
     <t xml:space="preserve"> Res2 61.8%</t>
   </si>
   <si>
-    <t>Commidity Channel Index(21)</t>
+    <t>Commodity Channel Index(21)</t>
   </si>
 </sst>
 </file>
@@ -602,27 +602,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="30">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="28">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1166,7 +1146,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="S2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AB251" sqref="AB251"/>
+      <selection pane="bottomRight" activeCell="AI2" sqref="AI2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42618,31 +42598,31 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="Q3:R251">
-    <cfRule type="cellIs" dxfId="29" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="36" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="37" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S3:X251">
-    <cfRule type="cellIs" dxfId="27" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="34" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="35" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P3:P251">
-    <cfRule type="containsText" dxfId="25" priority="32" operator="containsText" text="UP">
+    <cfRule type="containsText" dxfId="23" priority="32" operator="containsText" text="UP">
       <formula>NOT(ISERROR(SEARCH("UP",P3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="33" operator="containsText" text="down">
+    <cfRule type="containsText" dxfId="22" priority="33" operator="containsText" text="down">
       <formula>NOT(ISERROR(SEARCH("down",P3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE2:AE251">
-    <cfRule type="cellIs" dxfId="23" priority="31" operator="lessThan">
+    <cfRule type="cellIs" dxfId="21" priority="31" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -42657,25 +42637,25 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="29" operator="lessThan">
+    <cfRule type="cellIs" dxfId="20" priority="29" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="30" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="30" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T3:T251 R3:R251">
-    <cfRule type="containsText" dxfId="20" priority="28" operator="containsText" text="true">
+    <cfRule type="containsText" dxfId="18" priority="28" operator="containsText" text="true">
       <formula>NOT(ISERROR(SEARCH("true",R3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z2:Z251 AC2:AC251">
-    <cfRule type="containsText" dxfId="19" priority="27" operator="containsText" text="SELL">
+    <cfRule type="containsText" dxfId="17" priority="27" operator="containsText" text="SELL">
       <formula>NOT(ISERROR(SEARCH("SELL",Z2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y2:Y251 AB2:AB251">
-    <cfRule type="containsText" dxfId="18" priority="26" operator="containsText" text="buy">
+    <cfRule type="containsText" dxfId="16" priority="26" operator="containsText" text="buy">
       <formula>NOT(ISERROR(SEARCH("buy",Y2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -42692,55 +42672,55 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG4:AG251">
-    <cfRule type="containsText" dxfId="17" priority="19" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="15" priority="19" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",AG4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="2">
+    <cfRule type="containsText" dxfId="14" priority="20" operator="containsText" text="2">
       <formula>NOT(ISERROR(SEARCH("2",AG4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AT3:AT251">
-    <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="13" priority="18" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",AT3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ2:AJ251">
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="lessThan">
+    <cfRule type="cellIs" dxfId="12" priority="16" operator="lessThan">
       <formula>30</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="17" operator="greaterThan">
       <formula>70</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH2:AH251">
-    <cfRule type="cellIs" dxfId="12" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="15" operator="greaterThan">
       <formula>70</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="14" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="14" operator="lessThan">
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:R2">
-    <cfRule type="cellIs" dxfId="10" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:X2">
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2">
-    <cfRule type="containsText" dxfId="6" priority="5" operator="containsText" text="UP">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="UP">
       <formula>NOT(ISERROR(SEARCH("UP",P2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="down">
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="down">
       <formula>NOT(ISERROR(SEARCH("down",P2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -42755,15 +42735,15 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2 R2">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="true">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="true">
       <formula>NOT(ISERROR(SEARCH("true",R2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>